<commit_message>
update HKStock add function readIndexData
</commit_message>
<xml_diff>
--- a/HSC.xlsx
+++ b/HSC.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="273">
   <si>
     <t>ticker</t>
   </si>
@@ -824,6 +824,15 @@
   </si>
   <si>
     <t>2016-08-08</t>
+  </si>
+  <si>
+    <t>2016-08-09</t>
+  </si>
+  <si>
+    <t>2016-08-10</t>
+  </si>
+  <si>
+    <t>2016-08-11</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1190,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G264"/>
+  <dimension ref="A1:G267"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7256,6 +7265,75 @@
         <v>13473.79</v>
       </c>
     </row>
+    <row r="265" spans="1:7">
+      <c r="A265" s="1">
+        <v>263</v>
+      </c>
+      <c r="B265" t="s">
+        <v>6</v>
+      </c>
+      <c r="C265" t="s">
+        <v>270</v>
+      </c>
+      <c r="D265">
+        <v>13427.37</v>
+      </c>
+      <c r="E265">
+        <v>13419.69</v>
+      </c>
+      <c r="F265">
+        <v>13477.47</v>
+      </c>
+      <c r="G265">
+        <v>13459.27</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7">
+      <c r="A266" s="1">
+        <v>264</v>
+      </c>
+      <c r="B266" t="s">
+        <v>6</v>
+      </c>
+      <c r="C266" t="s">
+        <v>271</v>
+      </c>
+      <c r="D266">
+        <v>13453.64</v>
+      </c>
+      <c r="E266">
+        <v>13395.19</v>
+      </c>
+      <c r="F266">
+        <v>13532.5</v>
+      </c>
+      <c r="G266">
+        <v>13456.52</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7">
+      <c r="A267" s="1">
+        <v>265</v>
+      </c>
+      <c r="B267" t="s">
+        <v>6</v>
+      </c>
+      <c r="C267" t="s">
+        <v>272</v>
+      </c>
+      <c r="D267">
+        <v>13407.52</v>
+      </c>
+      <c r="E267">
+        <v>13367.43</v>
+      </c>
+      <c r="F267">
+        <v>13530.9</v>
+      </c>
+      <c r="G267">
+        <v>13453.74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>